<commit_message>
proses pembuatan laporan export
</commit_message>
<xml_diff>
--- a/public/selisihkurang.xlsx
+++ b/public/selisihkurang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\manonjaya\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50DEEFF-1317-4E3B-9C6E-52F89A8B247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDE1FFE-F1BE-420C-B51B-2C4DE68E4935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>04/01/2023</t>
   </si>
@@ -60,9 +60,6 @@
     <t>12/01/2023</t>
   </si>
   <si>
-    <t>SANDY BAYAR SELISIH KURANG SETORAN TGL 11/01/2023 ADM ASR</t>
-  </si>
-  <si>
     <t>SLAMET (SANDY) SELISIH KURANG SETORAN TGL 12/1/2023 ANGSURAN AN EDAH @SEWU</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>ARJUNA SELISIH KURANG SETORAN TGL 18/1/2023 SALAH JUMLAH MAJELIS KIMPULAN</t>
   </si>
   <si>
-    <t>19/01/2023</t>
-  </si>
-  <si>
-    <t>SANDY BAYAR SELISIH KURANG SETORAN TGL 12/1/2023</t>
-  </si>
-  <si>
     <t>23/01/2023</t>
   </si>
   <si>
@@ -90,31 +81,10 @@
     <t>24/01/2023</t>
   </si>
   <si>
-    <t>YOGI BAYAR SELISIH KURANG SETORAN TGL 12/01/2023</t>
-  </si>
-  <si>
     <t>YOGI SELISIH KURANG SETORAN TGL 24/01/2023</t>
   </si>
   <si>
-    <t>IQBAL BAYAR SELISIH KURANG</t>
-  </si>
-  <si>
     <t>25/01/2023</t>
-  </si>
-  <si>
-    <t>YOGI BAYAR SELISIH KURANG SETORAN TGL 24/01/2023</t>
-  </si>
-  <si>
-    <t>ARJUNA BAYAR SELISIH KURANG SETORAN TGL 23/01/2023</t>
-  </si>
-  <si>
-    <t>ARJUNA BAYAR SELISIH KURANG SETORAN TGL 18/01/2023</t>
-  </si>
-  <si>
-    <t>ARJUNA BAYAR SELISIH KURANG SETORAN TGL 09/01/2023</t>
-  </si>
-  <si>
-    <t>ARJUNA BAYAR SELISIH KURANG SETORAN TGL 04/01/2023</t>
   </si>
   <si>
     <t>ARJUNA SELISIH KURANG SETORAN TGL 25/01/2023</t>
@@ -490,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C1F922-485E-4E03-98AC-D03DED9B4038}">
-  <dimension ref="B1:F22"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -526,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -543,7 +513,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -560,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -577,16 +547,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="F5">
-        <v>18000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -594,13 +564,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6">
-        <v>25000</v>
+        <v>3000</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -608,16 +578,16 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -625,16 +595,16 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -642,33 +612,33 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F9">
-        <v>25000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10">
-        <v>500</v>
+        <v>6000</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -676,33 +646,33 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F11">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12">
-        <v>1000</v>
+        <v>38500</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -710,171 +680,18 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>16000</v>
       </c>
       <c r="F13">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>91000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19">
-        <v>6000</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20">
-        <v>2000</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21">
-        <v>38500</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22">
-        <v>16000</v>
-      </c>
-      <c r="F22">
         <v>0</v>
       </c>
     </row>

</xml_diff>